<commit_message>
Unificación de Metricas con RF-RNF
</commit_message>
<xml_diff>
--- a/Metricas.xlsx
+++ b/Metricas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\678855\Desktop\Prueba_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge Coronado\OneDrive\Escritorio\Prueba_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E65E2961-860C-4070-9297-34452BB9071B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE86B93-91D5-4383-8025-E8035AB33203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="4" xr2:uid="{4EB6F255-4A87-47BB-99FE-710E42CF0D44}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{4EB6F255-4A87-47BB-99FE-710E42CF0D44}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Densidad de defectos</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>Defectos</t>
+  </si>
+  <si>
+    <t>Mayor</t>
   </si>
 </sst>
 </file>
@@ -1067,9 +1070,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1107,7 +1110,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1213,7 +1216,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1355,7 +1358,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1471,9 +1474,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{695E72B0-3A6F-487B-92B5-098382B63208}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1483,7 +1486,7 @@
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1493,10 +1496,13 @@
       <c r="C1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f>(SUM($B2:$B5)/$C5)</f>
+        <f>(SUM($B2:$B5)/$D2)</f>
         <v>37.5</v>
       </c>
       <c r="B2">
@@ -1505,8 +1511,12 @@
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <f>MAX(C2:C5)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>20</v>
       </c>
@@ -1514,7 +1524,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>60</v>
       </c>
@@ -1522,7 +1532,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>30</v>
       </c>
@@ -1598,7 +1608,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7547FAE3-6D1B-40EE-A2DA-05D9792DF174}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>